<commit_message>
Update code after meeting
</commit_message>
<xml_diff>
--- a/raw_data/raw_excel/Crinita_Cala_Estreta_gen2017- feb2019.xlsx
+++ b/raw_data/raw_excel/Crinita_Cala_Estreta_gen2017- feb2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avipo\OneDrive - Danmarks Tekniske Universitet\Skrivebord\Postdoc\Projects\Fenology_cysto\raw_data\raw_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C75716C-EA09-49C7-93ED-2068329A98FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747C38D2-44F7-4591-9B68-568DF096DCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2790" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estructura de talles" sheetId="7" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3889" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="144">
   <si>
     <t>Date</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>sp = elegans</t>
   </si>
 </sst>
 </file>
@@ -4505,8 +4508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J134"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="G124" sqref="G124"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4635,6 +4638,9 @@
       </c>
       <c r="E6">
         <v>3</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -6555,8 +6561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F108" sqref="C2:F108"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8654,8 +8660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F102"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10717,7 +10723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A123" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -13755,8 +13761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K147"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F137"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16591,8 +16597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F106"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18790,7 +18796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:K137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A78" workbookViewId="0">
       <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
@@ -20900,8 +20906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23296,7 +23302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F125"/>
     </sheetView>
   </sheetViews>
@@ -25721,8 +25727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F108"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27869,7 +27875,7 @@
   <dimension ref="A1:J316"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -30568,8 +30574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F119"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32809,7 +32815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -35305,7 +35311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:J4"/>
     </sheetView>
   </sheetViews>
@@ -37144,8 +37150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F101"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38952,8 +38958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="H119" sqref="H119"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41036,8 +41042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F139"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43495,8 +43501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F95"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45206,7 +45212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J102"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -46357,8 +46363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F111"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>